<commit_message>
first steps on generatorification
</commit_message>
<xml_diff>
--- a/_append/data/text/equipment_generators.xlsx
+++ b/_append/data/text/equipment_generators.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dicey Dungeons\mods\morefluff\_append\data\text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Documents\DD Mods\MoreFluff\_append\data\text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD135B43-99B5-4E96-8495-FC36F50BCA18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19710" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19710" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="equipment_generators" sheetId="1" r:id="rId1"/>
@@ -20,205 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
-  <si>
-    <t>Idol of Blades</t>
-  </si>
-  <si>
-    <t>Flame Idol</t>
-  </si>
-  <si>
-    <t>Frost Idol</t>
-  </si>
-  <si>
-    <t>Chronal Idol</t>
-  </si>
-  <si>
-    <t>Idyllic Idol</t>
-  </si>
-  <si>
-    <t>Scrap Key</t>
-  </si>
-  <si>
-    <t>Volume Up</t>
-  </si>
-  <si>
-    <t>Chained Oak</t>
-  </si>
-  <si>
-    <t>Fuji</t>
-  </si>
-  <si>
-    <t>Chaffcannon</t>
-  </si>
-  <si>
-    <t>Medicine Practice</t>
-  </si>
-  <si>
-    <t>Spudge</t>
-  </si>
-  <si>
-    <t>Swoocerang</t>
-  </si>
-  <si>
-    <t>Keytar</t>
-  </si>
-  <si>
-    <t>Subduction</t>
-  </si>
-  <si>
-    <t>Dicesteal</t>
-  </si>
-  <si>
-    <t>Counter Charm</t>
-  </si>
-  <si>
-    <t>Theft and Shrubbery</t>
-  </si>
-  <si>
-    <t>Get Out Of Jail Free</t>
-  </si>
-  <si>
-    <t>Clank</t>
-  </si>
-  <si>
-    <t>Duplockate</t>
-  </si>
-  <si>
-    <t>Lockbash</t>
-  </si>
-  <si>
-    <t>Countdownerfeit</t>
-  </si>
-  <si>
-    <t>Roller Skates</t>
-  </si>
-  <si>
-    <t>Waltzer</t>
-  </si>
-  <si>
-    <t>Guillotine</t>
-  </si>
-  <si>
-    <t>Crypto Miner</t>
-  </si>
-  <si>
-    <t>Shattered Crown</t>
-  </si>
-  <si>
-    <t>Wispy Kaboom Smash</t>
-  </si>
-  <si>
-    <t>Glue Pact</t>
-  </si>
-  <si>
-    <t>Homemade Medal</t>
-  </si>
-  <si>
-    <t>Unlucky Shot</t>
-  </si>
-  <si>
-    <t>Sniper's Dream</t>
-  </si>
-  <si>
-    <t>Happy Camping</t>
-  </si>
-  <si>
-    <t>Throw The Book</t>
-  </si>
-  <si>
-    <t>Yeeteor</t>
-  </si>
-  <si>
-    <t>Broken Spell</t>
-  </si>
-  <si>
-    <t>Kleptolovania</t>
-  </si>
-  <si>
-    <t>Time Travel</t>
-  </si>
-  <si>
-    <t>Bolt Blaster</t>
-  </si>
-  <si>
-    <t>Power Pulse</t>
-  </si>
-  <si>
-    <t>MF Blank Equipment</t>
-  </si>
-  <si>
-    <t>Draining Bolt</t>
-  </si>
-  <si>
-    <t>Faeblade</t>
-  </si>
-  <si>
-    <t>Skeleglare</t>
-  </si>
-  <si>
-    <t>Ubersword</t>
-  </si>
-  <si>
-    <t>Morale Booster</t>
-  </si>
-  <si>
-    <t>Two Hookshots</t>
-  </si>
-  <si>
-    <t>Holy Heal Grenade</t>
-  </si>
-  <si>
-    <t>Sustained Loud Yelling</t>
-  </si>
-  <si>
-    <t>Shield of Light</t>
-  </si>
-  <si>
-    <t>Bumpster Sword</t>
-  </si>
-  <si>
-    <t>Ultimuplicate</t>
-  </si>
-  <si>
-    <t>Kablammo</t>
-  </si>
-  <si>
-    <t>Abracastabra</t>
-  </si>
-  <si>
-    <t>Second Sun</t>
-  </si>
-  <si>
-    <t>Eternal Frostbite</t>
-  </si>
-  <si>
-    <t>Hold The Line</t>
-  </si>
-  <si>
-    <t>Headache</t>
-  </si>
-  <si>
-    <t>Recurseion</t>
-  </si>
-  <si>
-    <t>Elementablast</t>
-  </si>
-  <si>
-    <t>Morphing Egg</t>
-  </si>
-  <si>
-    <t>Shadow Spell</t>
-  </si>
-  <si>
-    <t>Regen Spell</t>
-  </si>
-  <si>
-    <t>Blood Spell</t>
-  </si>
-  <si>
-    <t>Cancel</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Warrior</t>
   </si>
@@ -241,13 +42,19 @@
     <t>PU?</t>
   </si>
   <si>
-    <t>YES</t>
+    <t>BR exclusive?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1081,11 +888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,510 +900,36 @@
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>